<commit_message>
CentralCase Firmed up  -pre IRP cases
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/TCH_PWR_REL.xlsx
+++ b/SATIM/DataSpreadsheets/TCH_PWR_REL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9559B583-B157-4EA7-B2CB-CE717783C639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3460C40-9ED9-4E18-908A-30C9C54B9C4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1155" yWindow="-17655" windowWidth="27555" windowHeight="13575" activeTab="6" xr2:uid="{7C70B42E-9201-48A9-B8F0-1466C79FDCED}"/>
     <workbookView xWindow="570" yWindow="450" windowWidth="26880" windowHeight="13170" activeTab="4" xr2:uid="{C567A264-F0FD-49FD-BB9D-31E7FE2CFE51}"/>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="61">
   <si>
     <t>REGION1</t>
   </si>
@@ -4217,7 +4217,7 @@
       <selection activeCell="J10" sqref="J10:AP10"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7732,13 +7732,13 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:AP53"/>
+  <dimension ref="A1:AP54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10:AP10"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="A2" sqref="A2:XFD9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7894,16 +7894,16 @@
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -7912,92 +7912,178 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
-        <f t="shared" ref="A3:A24" si="1">IF(E3="","*","")</f>
-        <v/>
-      </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="str">
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A25" si="1">IF(E4="","*","")</f>
+        <v/>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="str">
         <f>ProcDataRM!B9</f>
         <v>ETCLECAMD-E</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3">
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4">
         <v>3</v>
       </c>
-      <c r="R3">
+      <c r="R4">
         <f>ProcDataRM!I9*31.536</f>
         <v>17.832588893756686</v>
       </c>
-      <c r="W3">
+      <c r="W4">
         <f>ProcDataRM!J9*31.536</f>
         <v>18.921600000000002</v>
       </c>
-      <c r="AB3">
+      <c r="AB4">
         <f>ProcDataRM!K9*31.536</f>
         <v>18.921600000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="str">
-        <f>ProcDataRM!B10</f>
-        <v>ETCLEGROO-E</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="R4">
-        <f>ProcDataRM!I10*31.536</f>
-        <v>12.1109044520399</v>
-      </c>
-      <c r="W4">
-        <f>ProcDataRM!J10*31.536</f>
-        <v>12.1109044520399</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.2">
@@ -8009,14 +8095,14 @@
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5" t="str">
-        <f>ProcDataRM!B11</f>
-        <v>ETCLEKOMA-E</v>
+        <f>ProcDataRM!B10</f>
+        <v>ETCLEGROO-E</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -8031,12 +8117,12 @@
         <v>3</v>
       </c>
       <c r="R5">
-        <f>ProcDataRM!I11*31.536</f>
-        <v>11.179500765531754</v>
+        <f>ProcDataRM!I10*31.536</f>
+        <v>12.1109044520399</v>
       </c>
       <c r="W5">
-        <f>ProcDataRM!J11*31.536</f>
-        <v>11.179500765531754</v>
+        <f>ProcDataRM!J10*31.536</f>
+        <v>12.1109044520399</v>
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.2">
@@ -8048,14 +8134,14 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
       <c r="E6" t="str">
-        <f>ProcDataRM!B12</f>
-        <v>ETCLEARNO-E</v>
+        <f>ProcDataRM!B11</f>
+        <v>ETCLEKOMA-E</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -8070,16 +8156,12 @@
         <v>3</v>
       </c>
       <c r="R6">
-        <f>ProcDataRM!I12*31.536</f>
-        <v>17.433755987040588</v>
+        <f>ProcDataRM!I11*31.536</f>
+        <v>11.179500765531754</v>
       </c>
       <c r="W6">
-        <f>ProcDataRM!J12*31.536</f>
-        <v>20.656080000000003</v>
-      </c>
-      <c r="AB6">
-        <f>ProcDataRM!K12*31.536</f>
-        <v>17.212348800000001</v>
+        <f>ProcDataRM!J11*31.536</f>
+        <v>11.179500765531754</v>
       </c>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.2">
@@ -8091,14 +8173,14 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
       <c r="E7" t="str">
-        <f>ProcDataRM!B13</f>
-        <v>ETCLEDUVH-E</v>
+        <f>ProcDataRM!B12</f>
+        <v>ETCLEARNO-E</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -8113,16 +8195,16 @@
         <v>3</v>
       </c>
       <c r="R7">
-        <f>ProcDataRM!I13*31.536</f>
-        <v>18.099885160251002</v>
+        <f>ProcDataRM!I12*31.536</f>
+        <v>17.433755987040588</v>
       </c>
       <c r="W7">
-        <f>ProcDataRM!J13*31.536</f>
-        <v>19.274803200000001</v>
+        <f>ProcDataRM!J12*31.536</f>
+        <v>20.656080000000003</v>
       </c>
       <c r="AB7">
-        <f>ProcDataRM!K13*31.536</f>
-        <v>18.987825600000001</v>
+        <f>ProcDataRM!K12*31.536</f>
+        <v>17.212348800000001</v>
       </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.2">
@@ -8134,14 +8216,14 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
       </c>
       <c r="E8" t="str">
-        <f>ProcDataRM!B14</f>
-        <v>ETCLEHEND-E</v>
+        <f>ProcDataRM!B13</f>
+        <v>ETCLEDUVH-E</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -8156,12 +8238,16 @@
         <v>3</v>
       </c>
       <c r="R8">
-        <f>ProcDataRM!I14*31.536</f>
-        <v>18.317678013302608</v>
+        <f>ProcDataRM!I13*31.536</f>
+        <v>18.099885160251002</v>
       </c>
       <c r="W8">
-        <f>ProcDataRM!J14*31.536</f>
-        <v>19.2148848</v>
+        <f>ProcDataRM!J13*31.536</f>
+        <v>19.274803200000001</v>
+      </c>
+      <c r="AB8">
+        <f>ProcDataRM!K13*31.536</f>
+        <v>18.987825600000001</v>
       </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.2">
@@ -8173,14 +8259,14 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
       </c>
       <c r="E9" t="str">
-        <f>ProcDataRM!B15</f>
-        <v>ETCLEKEND-E</v>
+        <f>ProcDataRM!B14</f>
+        <v>ETCLEHEND-E</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
@@ -8195,16 +8281,12 @@
         <v>3</v>
       </c>
       <c r="R9">
-        <f>ProcDataRM!I15*31.536</f>
-        <v>24.360517923566423</v>
+        <f>ProcDataRM!I14*31.536</f>
+        <v>18.317678013302608</v>
       </c>
       <c r="W9">
-        <f>ProcDataRM!J15*31.536</f>
-        <v>23.380790399999999</v>
-      </c>
-      <c r="AB9">
-        <f>ProcDataRM!K15*31.536</f>
-        <v>23.002358400000002</v>
+        <f>ProcDataRM!J14*31.536</f>
+        <v>19.2148848</v>
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.2">
@@ -8216,14 +8298,14 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
       </c>
       <c r="E10" t="str">
-        <f>ProcDataRM!B16</f>
-        <v>ETCLEKRIE-E</v>
+        <f>ProcDataRM!B15</f>
+        <v>ETCLEKEND-E</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -8238,16 +8320,16 @@
         <v>3</v>
       </c>
       <c r="R10">
-        <f>ProcDataRM!I16*31.536</f>
-        <v>16.948259039814825</v>
+        <f>ProcDataRM!I15*31.536</f>
+        <v>24.360517923566423</v>
       </c>
       <c r="W10">
-        <f>ProcDataRM!J16*31.536</f>
-        <v>20.321798399999999</v>
+        <f>ProcDataRM!J15*31.536</f>
+        <v>23.380790399999999</v>
       </c>
       <c r="AB10">
-        <f>ProcDataRM!K16*31.536</f>
-        <v>20.230343999999999</v>
+        <f>ProcDataRM!K15*31.536</f>
+        <v>23.002358400000002</v>
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.2">
@@ -8259,14 +8341,14 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
       </c>
       <c r="E11" t="str">
-        <f>ProcDataRM!B17</f>
-        <v>ETCLELETH-E</v>
+        <f>ProcDataRM!B16</f>
+        <v>ETCLEKRIE-E</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
@@ -8281,16 +8363,16 @@
         <v>3</v>
       </c>
       <c r="R11">
-        <f>ProcDataRM!I17*31.536</f>
-        <v>20.309935056133526</v>
+        <f>ProcDataRM!I16*31.536</f>
+        <v>16.948259039814825</v>
       </c>
       <c r="W11">
-        <f>ProcDataRM!J17*31.536</f>
-        <v>23.6141568</v>
+        <f>ProcDataRM!J16*31.536</f>
+        <v>20.321798399999999</v>
       </c>
       <c r="AB11">
-        <f>ProcDataRM!K17*31.536</f>
-        <v>22.368484800000001</v>
+        <f>ProcDataRM!K16*31.536</f>
+        <v>20.230343999999999</v>
       </c>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.2">
@@ -8302,14 +8384,14 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
       </c>
       <c r="E12" t="str">
-        <f>ProcDataRM!B18</f>
-        <v>ETCLEMAJD-E</v>
+        <f>ProcDataRM!B17</f>
+        <v>ETCLELETH-E</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
@@ -8324,15 +8406,15 @@
         <v>3</v>
       </c>
       <c r="R12">
-        <f>ProcDataRM!I18*31.536</f>
-        <v>23.025442410053383</v>
+        <f>ProcDataRM!I17*31.536</f>
+        <v>20.309935056133526</v>
       </c>
       <c r="W12">
-        <f>ProcDataRM!J18*31.536</f>
-        <v>24.282720000000001</v>
+        <f>ProcDataRM!J17*31.536</f>
+        <v>23.6141568</v>
       </c>
       <c r="AB12">
-        <f>ProcDataRM!K18*31.536</f>
+        <f>ProcDataRM!K17*31.536</f>
         <v>22.368484800000001</v>
       </c>
     </row>
@@ -8345,14 +8427,14 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
       </c>
       <c r="E13" t="str">
-        <f>ProcDataRM!B19</f>
-        <v>ETCLEMAJW-E</v>
+        <f>ProcDataRM!B18</f>
+        <v>ETCLEMAJD-E</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -8367,15 +8449,15 @@
         <v>3</v>
       </c>
       <c r="R13">
-        <f>ProcDataRM!I19*31.536</f>
+        <f>ProcDataRM!I18*31.536</f>
         <v>23.025442410053383</v>
       </c>
       <c r="W13">
-        <f>ProcDataRM!J19*31.536</f>
+        <f>ProcDataRM!J18*31.536</f>
         <v>24.282720000000001</v>
       </c>
       <c r="AB13">
-        <f>ProcDataRM!K19*31.536</f>
+        <f>ProcDataRM!K18*31.536</f>
         <v>22.368484800000001</v>
       </c>
     </row>
@@ -8388,14 +8470,14 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
       </c>
       <c r="E14" t="str">
-        <f>ProcDataRM!B20</f>
-        <v>ETCLEMATI-E</v>
+        <f>ProcDataRM!B19</f>
+        <v>ETCLEMAJW-E</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
@@ -8410,16 +8492,16 @@
         <v>3</v>
       </c>
       <c r="R14">
-        <f>ProcDataRM!I20*31.536</f>
-        <v>26.062559024390243</v>
+        <f>ProcDataRM!I19*31.536</f>
+        <v>23.025442410053383</v>
       </c>
       <c r="W14">
-        <f>ProcDataRM!J20*31.536</f>
-        <v>24.7147632</v>
+        <f>ProcDataRM!J19*31.536</f>
+        <v>24.282720000000001</v>
       </c>
       <c r="AB14">
-        <f>ProcDataRM!K20*31.536</f>
-        <v>25.042737600000002</v>
+        <f>ProcDataRM!K19*31.536</f>
+        <v>22.368484800000001</v>
       </c>
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.2">
@@ -8431,14 +8513,14 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
       </c>
       <c r="E15" t="str">
-        <f>ProcDataRM!B21</f>
-        <v>ETCLEMATL-E</v>
+        <f>ProcDataRM!B20</f>
+        <v>ETCLEMATI-E</v>
       </c>
       <c r="F15" t="s">
         <v>11</v>
@@ -8453,16 +8535,16 @@
         <v>3</v>
       </c>
       <c r="R15">
-        <f>ProcDataRM!I21*31.536</f>
-        <v>21.321016073062601</v>
+        <f>ProcDataRM!I20*31.536</f>
+        <v>26.062559024390243</v>
       </c>
       <c r="W15">
-        <f>ProcDataRM!J21*31.536</f>
-        <v>22.242340800000001</v>
+        <f>ProcDataRM!J20*31.536</f>
+        <v>24.7147632</v>
       </c>
       <c r="AB15">
-        <f>ProcDataRM!K21*31.536</f>
-        <v>21.9995136</v>
+        <f>ProcDataRM!K20*31.536</f>
+        <v>25.042737600000002</v>
       </c>
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.2">
@@ -8474,14 +8556,14 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
       </c>
       <c r="E16" t="str">
-        <f>ProcDataRM!B22</f>
-        <v>ETCLETUTU-E</v>
+        <f>ProcDataRM!B21</f>
+        <v>ETCLEMATL-E</v>
       </c>
       <c r="F16" t="s">
         <v>11</v>
@@ -8496,16 +8578,16 @@
         <v>3</v>
       </c>
       <c r="R16">
-        <f>ProcDataRM!I22*31.536</f>
-        <v>17.733482821612462</v>
+        <f>ProcDataRM!I21*31.536</f>
+        <v>21.321016073062601</v>
       </c>
       <c r="W16">
-        <f>ProcDataRM!J22*31.536</f>
-        <v>19.284264000000004</v>
+        <f>ProcDataRM!J21*31.536</f>
+        <v>22.242340800000001</v>
       </c>
       <c r="AB16">
-        <f>ProcDataRM!K22*31.536</f>
-        <v>18.316108799999999</v>
+        <f>ProcDataRM!K21*31.536</f>
+        <v>21.9995136</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
@@ -8517,14 +8599,14 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
         <v>16</v>
       </c>
       <c r="E17" t="str">
-        <f>ProcDataRM!B23</f>
-        <v>ETCLEKELB-E</v>
+        <f>ProcDataRM!B22</f>
+        <v>ETCLETUTU-E</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
@@ -8539,8 +8621,16 @@
         <v>3</v>
       </c>
       <c r="R17">
-        <f>ProcDataRM!I23*31.536</f>
-        <v>10.242569999999999</v>
+        <f>ProcDataRM!I22*31.536</f>
+        <v>17.733482821612462</v>
+      </c>
+      <c r="W17">
+        <f>ProcDataRM!J22*31.536</f>
+        <v>19.284264000000004</v>
+      </c>
+      <c r="AB17">
+        <f>ProcDataRM!K22*31.536</f>
+        <v>18.316108799999999</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
@@ -8552,14 +8642,14 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
         <v>16</v>
       </c>
       <c r="E18" t="str">
-        <f>ProcDataRM!B24</f>
-        <v>ETCLEPFSS-E</v>
+        <f>ProcDataRM!B23</f>
+        <v>ETCLEKELB-E</v>
       </c>
       <c r="F18" t="s">
         <v>11</v>
@@ -8574,16 +8664,8 @@
         <v>3</v>
       </c>
       <c r="R18">
-        <f>ProcDataRM!I24*31.536</f>
-        <v>23.078752275543476</v>
-      </c>
-      <c r="W18">
-        <f>ProcDataRM!J24*31.536</f>
-        <v>23.078752275543476</v>
-      </c>
-      <c r="AB18">
-        <f>ProcDataRM!K24*31.536</f>
-        <v>23.078752275543476</v>
+        <f>ProcDataRM!I23*31.536</f>
+        <v>10.242569999999999</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
@@ -8595,14 +8677,14 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
         <v>16</v>
       </c>
       <c r="E19" t="str">
-        <f>ProcDataRM!B25</f>
-        <v>ETCLEPFSI-E</v>
+        <f>ProcDataRM!B24</f>
+        <v>ETCLEPFSS-E</v>
       </c>
       <c r="F19" t="s">
         <v>11</v>
@@ -8617,16 +8699,16 @@
         <v>3</v>
       </c>
       <c r="R19">
-        <f>ProcDataRM!I25*31.536</f>
-        <v>17.561821021874998</v>
+        <f>ProcDataRM!I24*31.536</f>
+        <v>23.078752275543476</v>
       </c>
       <c r="W19">
-        <f>ProcDataRM!J25*31.536</f>
-        <v>17.561821021874998</v>
+        <f>ProcDataRM!J24*31.536</f>
+        <v>23.078752275543476</v>
       </c>
       <c r="AB19">
-        <f>ProcDataRM!K25*31.536</f>
-        <v>17.561821021874998</v>
+        <f>ProcDataRM!K24*31.536</f>
+        <v>23.078752275543476</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
@@ -8638,14 +8720,14 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
       </c>
       <c r="E20" t="str">
-        <f>ProcDataRM!B26</f>
-        <v>ETODSGT-E</v>
+        <f>ProcDataRM!B25</f>
+        <v>ETCLEPFSI-E</v>
       </c>
       <c r="F20" t="s">
         <v>11</v>
@@ -8660,16 +8742,16 @@
         <v>3</v>
       </c>
       <c r="R20">
-        <f>ProcDataRM!I26*31.536</f>
-        <v>1.5768000000000002</v>
+        <f>ProcDataRM!I25*31.536</f>
+        <v>17.561821021874998</v>
       </c>
       <c r="W20">
-        <f>ProcDataRM!J26*31.536</f>
-        <v>1.5768000000000002</v>
+        <f>ProcDataRM!J25*31.536</f>
+        <v>17.561821021874998</v>
       </c>
       <c r="AB20">
-        <f>ProcDataRM!K26*31.536</f>
-        <v>1.5768000000000002</v>
+        <f>ProcDataRM!K25*31.536</f>
+        <v>17.561821021874998</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
@@ -8681,14 +8763,14 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
         <v>16</v>
       </c>
       <c r="E21" t="str">
-        <f>ProcDataRM!B27</f>
-        <v>ERHYD-E</v>
+        <f>ProcDataRM!B26</f>
+        <v>ETODSGT-E</v>
       </c>
       <c r="F21" t="s">
         <v>11</v>
@@ -8703,16 +8785,16 @@
         <v>3</v>
       </c>
       <c r="R21">
-        <f>ProcDataRM!I27*31.536</f>
-        <v>3.7848586466165415</v>
+        <f>ProcDataRM!I26*31.536</f>
+        <v>1.5768000000000002</v>
       </c>
       <c r="W21">
-        <f>ProcDataRM!J27*31.536</f>
-        <v>3.7848586466165415</v>
+        <f>ProcDataRM!J26*31.536</f>
+        <v>1.5768000000000002</v>
       </c>
       <c r="AB21">
-        <f>ProcDataRM!K27*31.536</f>
-        <v>3.7848586466165415</v>
+        <f>ProcDataRM!K26*31.536</f>
+        <v>1.5768000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
@@ -8724,14 +8806,14 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
         <v>16</v>
       </c>
       <c r="E22" t="str">
-        <f>ProcDataRM!B28</f>
-        <v>ERHYD-I</v>
+        <f>ProcDataRM!B27</f>
+        <v>ERHYD-E</v>
       </c>
       <c r="F22" t="s">
         <v>11</v>
@@ -8746,8 +8828,16 @@
         <v>3</v>
       </c>
       <c r="R22">
-        <f>ProcDataRM!I28*31.536</f>
-        <v>21.755728800000004</v>
+        <f>ProcDataRM!I27*31.536</f>
+        <v>3.7848586466165415</v>
+      </c>
+      <c r="W22">
+        <f>ProcDataRM!J27*31.536</f>
+        <v>3.7848586466165415</v>
+      </c>
+      <c r="AB22">
+        <f>ProcDataRM!K27*31.536</f>
+        <v>3.7848586466165415</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
@@ -8759,14 +8849,14 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
         <v>16</v>
       </c>
       <c r="E23" t="str">
-        <f>ProcDataRM!B29</f>
-        <v>ETNUC-E</v>
+        <f>ProcDataRM!B28</f>
+        <v>ERHYD-I</v>
       </c>
       <c r="F23" t="s">
         <v>11</v>
@@ -8781,16 +8871,8 @@
         <v>3</v>
       </c>
       <c r="R23">
-        <f>ProcDataRM!I29*31.536</f>
-        <v>29.202929032258066</v>
-      </c>
-      <c r="W23">
-        <f>ProcDataRM!J29*31.536</f>
-        <v>26.540697600000001</v>
-      </c>
-      <c r="AB23">
-        <f>ProcDataRM!K29*31.536</f>
-        <v>26.540697600000001</v>
+        <f>ProcDataRM!I28*31.536</f>
+        <v>21.755728800000004</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
@@ -8802,46 +8884,58 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
       </c>
       <c r="E24" t="str">
+        <f>ProcDataRM!B29</f>
+        <v>ETNUC-E</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="R24">
+        <f>ProcDataRM!I29*31.536</f>
+        <v>29.202929032258066</v>
+      </c>
+      <c r="W24">
+        <f>ProcDataRM!J29*31.536</f>
+        <v>26.540697600000001</v>
+      </c>
+      <c r="AB24">
+        <f>ProcDataRM!K29*31.536</f>
+        <v>26.540697600000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="str">
         <f>ProcDataRM!B30</f>
         <v>EPTSTO-E</v>
       </c>
-      <c r="F24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A25" t="str">
-        <f>IF(E25="","*","")</f>
-        <v>*</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" t="str">
-        <f>ProcDataRM!B31</f>
-        <v/>
-      </c>
       <c r="F25" t="s">
         <v>11</v>
       </c>
@@ -8857,87 +8951,75 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
-        <f t="shared" ref="A26:A65" si="2">IF(E26="","*","")</f>
-        <v/>
+        <f>IF(E26="","*","")</f>
+        <v>*</v>
       </c>
       <c r="B26" t="s">
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
       </c>
       <c r="E26" t="str">
+        <f>ProcDataRM!B31</f>
+        <v/>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A27" t="str">
+        <f t="shared" ref="A27:A66" si="2">IF(E27="","*","")</f>
+        <v/>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" t="str">
         <f>ProcDataRM!B32</f>
         <v>ETCLEMEDU-N</v>
       </c>
-      <c r="F26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" t="s">
-        <v>11</v>
-      </c>
-      <c r="I26">
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27">
         <v>3</v>
       </c>
-      <c r="R26">
+      <c r="R27">
         <f>ProcDataRM!I32*31.536</f>
         <v>17.674461745787703</v>
       </c>
-      <c r="W26">
+      <c r="W27">
         <f>ProcDataRM!J32*31.536</f>
         <v>25.228800000000003</v>
       </c>
-      <c r="AB26">
+      <c r="AB27">
         <f>ProcDataRM!K32*31.536</f>
-        <v>25.228800000000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A27" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" t="str">
-        <f>ProcDataRM!B33</f>
-        <v>ETCLEKUSI-N</v>
-      </c>
-      <c r="F27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27">
-        <v>3</v>
-      </c>
-      <c r="R27">
-        <f>ProcDataRM!I33*31.536</f>
-        <v>17.674461745787703</v>
-      </c>
-      <c r="W27">
-        <f>ProcDataRM!J33*31.536</f>
-        <v>25.228800000000003</v>
-      </c>
-      <c r="AB27">
-        <f>ProcDataRM!K33*31.536</f>
         <v>25.228800000000003</v>
       </c>
     </row>
@@ -8950,14 +9032,14 @@
         <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
         <v>16</v>
       </c>
       <c r="E28" t="str">
-        <f>ProcDataRM!B34</f>
-        <v>ETCLEWATE-N</v>
+        <f>ProcDataRM!B33</f>
+        <v>ETCLEKUSI-N</v>
       </c>
       <c r="F28" t="s">
         <v>11</v>
@@ -8972,7 +9054,15 @@
         <v>3</v>
       </c>
       <c r="R28">
-        <f>ProcDataRM!I34*31.536</f>
+        <f>ProcDataRM!I33*31.536</f>
+        <v>17.674461745787703</v>
+      </c>
+      <c r="W28">
+        <f>ProcDataRM!J33*31.536</f>
+        <v>25.228800000000003</v>
+      </c>
+      <c r="AB28">
+        <f>ProcDataRM!K33*31.536</f>
         <v>25.228800000000003</v>
       </c>
     </row>
@@ -8985,14 +9075,14 @@
         <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D29" t="s">
         <v>16</v>
       </c>
       <c r="E29" t="str">
-        <f>ProcDataRM!B35</f>
-        <v>EPTSTO-N</v>
+        <f>ProcDataRM!B34</f>
+        <v>ETCLEWATE-N</v>
       </c>
       <c r="F29" t="s">
         <v>11</v>
@@ -9005,6 +9095,10 @@
       </c>
       <c r="I29">
         <v>3</v>
+      </c>
+      <c r="R29">
+        <f>ProcDataRM!I34*31.536</f>
+        <v>25.228800000000003</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
@@ -9016,14 +9110,14 @@
         <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
         <v>16</v>
       </c>
       <c r="E30" t="str">
-        <f>ProcDataRM!B36</f>
-        <v>ETODSGT-N</v>
+        <f>ProcDataRM!B35</f>
+        <v>EPTSTO-N</v>
       </c>
       <c r="F30" t="s">
         <v>11</v>
@@ -9036,18 +9130,6 @@
       </c>
       <c r="I30">
         <v>3</v>
-      </c>
-      <c r="R30">
-        <f>ProcDataRM!I36*31.536</f>
-        <v>1.5768000000000002</v>
-      </c>
-      <c r="W30">
-        <f>ProcDataRM!J36*31.536</f>
-        <v>1.5768000000000002</v>
-      </c>
-      <c r="AB30">
-        <f>ProcDataRM!K36*31.536</f>
-        <v>1.5768000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
@@ -9059,14 +9141,14 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D31" t="s">
         <v>16</v>
       </c>
       <c r="E31" t="str">
-        <f>ProcDataRM!B37</f>
-        <v>ETCLDFB-N</v>
+        <f>ProcDataRM!B36</f>
+        <v>ETODSGT-N</v>
       </c>
       <c r="F31" t="s">
         <v>11</v>
@@ -9081,16 +9163,16 @@
         <v>3</v>
       </c>
       <c r="R31">
-        <f>ProcDataRM!I37*31.536</f>
-        <v>25.228800000000003</v>
+        <f>ProcDataRM!I36*31.536</f>
+        <v>1.5768000000000002</v>
       </c>
       <c r="W31">
-        <f>ProcDataRM!J37*31.536</f>
-        <v>25.228800000000003</v>
+        <f>ProcDataRM!J36*31.536</f>
+        <v>1.5768000000000002</v>
       </c>
       <c r="AB31">
-        <f>ProcDataRM!K37*31.536</f>
-        <v>25.228800000000003</v>
+        <f>ProcDataRM!K36*31.536</f>
+        <v>1.5768000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
@@ -9102,14 +9184,14 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D32" t="s">
         <v>16</v>
       </c>
       <c r="E32" t="str">
-        <f>ProcDataRM!B38</f>
-        <v>ERHYD-N</v>
+        <f>ProcDataRM!B37</f>
+        <v>ETCLDFB-N</v>
       </c>
       <c r="F32" t="s">
         <v>11</v>
@@ -9122,6 +9204,18 @@
       </c>
       <c r="I32">
         <v>3</v>
+      </c>
+      <c r="R32">
+        <f>ProcDataRM!I37*31.536</f>
+        <v>25.228800000000003</v>
+      </c>
+      <c r="W32">
+        <f>ProcDataRM!J37*31.536</f>
+        <v>25.228800000000003</v>
+      </c>
+      <c r="AB32">
+        <f>ProcDataRM!K37*31.536</f>
+        <v>25.228800000000003</v>
       </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.2">
@@ -9133,14 +9227,14 @@
         <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D33" t="s">
         <v>16</v>
       </c>
       <c r="E33" t="str">
-        <f>ProcDataRM!B39</f>
-        <v>ETNUC-N</v>
+        <f>ProcDataRM!B38</f>
+        <v>ERHYD-N</v>
       </c>
       <c r="F33" t="s">
         <v>11</v>
@@ -9153,18 +9247,6 @@
       </c>
       <c r="I33">
         <v>3</v>
-      </c>
-      <c r="R33">
-        <f>ProcDataRM!I39*31.536</f>
-        <v>26.805600000000002</v>
-      </c>
-      <c r="W33">
-        <f>ProcDataRM!J39*31.536</f>
-        <v>26.805600000000002</v>
-      </c>
-      <c r="AB33">
-        <f>ProcDataRM!K39*31.536</f>
-        <v>26.805600000000002</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.2">
@@ -9176,14 +9258,14 @@
         <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D34" t="s">
         <v>16</v>
       </c>
       <c r="E34" t="str">
-        <f>ProcDataRM!B40</f>
-        <v>ERSOLTC09-N</v>
+        <f>ProcDataRM!B39</f>
+        <v>ETNUC-N</v>
       </c>
       <c r="F34" t="s">
         <v>11</v>
@@ -9198,16 +9280,16 @@
         <v>3</v>
       </c>
       <c r="R34">
-        <f>ProcDataRM!I40*31.536</f>
-        <v>14.758225290144003</v>
+        <f>ProcDataRM!I39*31.536</f>
+        <v>26.805600000000002</v>
       </c>
       <c r="W34">
-        <f>ProcDataRM!J40*31.536</f>
-        <v>14.758225290144003</v>
+        <f>ProcDataRM!J39*31.536</f>
+        <v>26.805600000000002</v>
       </c>
       <c r="AB34">
-        <f>ProcDataRM!K40*31.536</f>
-        <v>14.758225290144003</v>
+        <f>ProcDataRM!K39*31.536</f>
+        <v>26.805600000000002</v>
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.2">
@@ -9219,14 +9301,14 @@
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D35" t="s">
         <v>16</v>
       </c>
       <c r="E35" t="str">
-        <f>ProcDataRM!B41</f>
-        <v>ERSOLPCF-N</v>
+        <f>ProcDataRM!B40</f>
+        <v>ERSOLTC09-N</v>
       </c>
       <c r="F35" t="s">
         <v>11</v>
@@ -9241,16 +9323,16 @@
         <v>3</v>
       </c>
       <c r="R35">
-        <f>ProcDataRM!I41*31.536</f>
-        <v>7.8840448126560005</v>
+        <f>ProcDataRM!I40*31.536</f>
+        <v>14.758225290144003</v>
       </c>
       <c r="W35">
-        <f>ProcDataRM!J41*31.536</f>
-        <v>7.8840448126560005</v>
+        <f>ProcDataRM!J40*31.536</f>
+        <v>14.758225290144003</v>
       </c>
       <c r="AB35">
-        <f>ProcDataRM!K41*31.536</f>
-        <v>7.8840448126560005</v>
+        <f>ProcDataRM!K40*31.536</f>
+        <v>14.758225290144003</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.2">
@@ -9262,14 +9344,14 @@
         <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D36" t="s">
         <v>16</v>
       </c>
       <c r="E36" t="str">
-        <f>ProcDataRM!B42</f>
-        <v>ERSOLPCT-N</v>
+        <f>ProcDataRM!B41</f>
+        <v>ERSOLPCF-N</v>
       </c>
       <c r="F36" t="s">
         <v>11</v>
@@ -9284,16 +9366,16 @@
         <v>3</v>
       </c>
       <c r="R36">
-        <f>ProcDataRM!I42*31.536</f>
-        <v>8.8300941596640019</v>
+        <f>ProcDataRM!I41*31.536</f>
+        <v>7.8840448126560005</v>
       </c>
       <c r="W36">
-        <f>ProcDataRM!J42*31.536</f>
-        <v>8.8300941596640019</v>
+        <f>ProcDataRM!J41*31.536</f>
+        <v>7.8840448126560005</v>
       </c>
       <c r="AB36">
-        <f>ProcDataRM!K42*31.536</f>
-        <v>8.8300941596640019</v>
+        <f>ProcDataRM!K41*31.536</f>
+        <v>7.8840448126560005</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.2">
@@ -9305,14 +9387,14 @@
         <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D37" t="s">
         <v>16</v>
       </c>
       <c r="E37" t="str">
-        <f>ProcDataRM!B43</f>
-        <v>ERWNDH-N</v>
+        <f>ProcDataRM!B42</f>
+        <v>ERSOLPCT-N</v>
       </c>
       <c r="F37" t="s">
         <v>11</v>
@@ -9327,16 +9409,16 @@
         <v>3</v>
       </c>
       <c r="R37">
-        <f>ProcDataRM!I43*31.536</f>
-        <v>11.818439244000002</v>
+        <f>ProcDataRM!I42*31.536</f>
+        <v>8.8300941596640019</v>
       </c>
       <c r="W37">
-        <f>ProcDataRM!J43*31.536</f>
-        <v>12.196770044976001</v>
+        <f>ProcDataRM!J42*31.536</f>
+        <v>8.8300941596640019</v>
       </c>
       <c r="AB37">
-        <f>ProcDataRM!K43*31.536</f>
-        <v>12.575100845951999</v>
+        <f>ProcDataRM!K42*31.536</f>
+        <v>8.8300941596640019</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.2">
@@ -9348,14 +9430,14 @@
         <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D38" t="s">
         <v>16</v>
       </c>
       <c r="E38" t="str">
-        <f>ProcDataRM!B44</f>
-        <v>ERHYDGIW-I</v>
+        <f>ProcDataRM!B43</f>
+        <v>ERWNDH-N</v>
       </c>
       <c r="F38" t="s">
         <v>11</v>
@@ -9370,16 +9452,16 @@
         <v>3</v>
       </c>
       <c r="R38">
-        <f>ProcDataRM!I44*31.536</f>
-        <v>24.598080000000003</v>
+        <f>ProcDataRM!I43*31.536</f>
+        <v>11.818439244000002</v>
       </c>
       <c r="W38">
-        <f>ProcDataRM!J44*31.536</f>
-        <v>24.598080000000003</v>
+        <f>ProcDataRM!J43*31.536</f>
+        <v>12.196770044976001</v>
       </c>
       <c r="AB38">
-        <f>ProcDataRM!K44*31.536</f>
-        <v>24.598080000000003</v>
+        <f>ProcDataRM!K43*31.536</f>
+        <v>12.575100845951999</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.2">
@@ -9391,14 +9473,14 @@
         <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D39" t="s">
         <v>16</v>
       </c>
       <c r="E39" t="str">
-        <f>ProcDataRM!B45</f>
-        <v>ETGICGT-N</v>
+        <f>ProcDataRM!B44</f>
+        <v>ERHYDGIW-I</v>
       </c>
       <c r="F39" t="s">
         <v>11</v>
@@ -9413,16 +9495,16 @@
         <v>3</v>
       </c>
       <c r="R39">
-        <f>ProcDataRM!I45*31.536</f>
-        <v>3.1536000000000004</v>
+        <f>ProcDataRM!I44*31.536</f>
+        <v>24.598080000000003</v>
       </c>
       <c r="W39">
-        <f>ProcDataRM!J45*31.536</f>
-        <v>3.1536000000000004</v>
+        <f>ProcDataRM!J44*31.536</f>
+        <v>24.598080000000003</v>
       </c>
       <c r="AB39">
-        <f>ProcDataRM!K45*31.536</f>
-        <v>3.1536000000000004</v>
+        <f>ProcDataRM!K44*31.536</f>
+        <v>24.598080000000003</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.2">
@@ -9434,14 +9516,14 @@
         <v>23</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D40" t="s">
         <v>16</v>
       </c>
       <c r="E40" t="str">
-        <f>ProcDataRM!B46</f>
-        <v>ETGICCC-N</v>
+        <f>ProcDataRM!B45</f>
+        <v>ETGICGT-N</v>
       </c>
       <c r="F40" t="s">
         <v>11</v>
@@ -9456,16 +9538,16 @@
         <v>3</v>
       </c>
       <c r="R40">
-        <f>ProcDataRM!I46*31.536</f>
-        <v>15.768000000000001</v>
+        <f>ProcDataRM!I45*31.536</f>
+        <v>3.1536000000000004</v>
       </c>
       <c r="W40">
-        <f>ProcDataRM!J46*31.536</f>
-        <v>15.768000000000001</v>
+        <f>ProcDataRM!J45*31.536</f>
+        <v>3.1536000000000004</v>
       </c>
       <c r="AB40">
-        <f>ProcDataRM!K46*31.536</f>
-        <v>15.768000000000001</v>
+        <f>ProcDataRM!K45*31.536</f>
+        <v>3.1536000000000004</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.2">
@@ -9477,14 +9559,14 @@
         <v>23</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D41" t="s">
         <v>16</v>
       </c>
       <c r="E41" t="str">
-        <f>ProcDataRM!B47</f>
-        <v>ETGICEN-N</v>
+        <f>ProcDataRM!B46</f>
+        <v>ETGICCC-N</v>
       </c>
       <c r="F41" t="s">
         <v>11</v>
@@ -9499,15 +9581,15 @@
         <v>3</v>
       </c>
       <c r="R41">
-        <f>ProcDataRM!I47*31.536</f>
+        <f>ProcDataRM!I46*31.536</f>
         <v>15.768000000000001</v>
       </c>
       <c r="W41">
-        <f>ProcDataRM!J47*31.536</f>
+        <f>ProcDataRM!J46*31.536</f>
         <v>15.768000000000001</v>
       </c>
       <c r="AB41">
-        <f>ProcDataRM!K47*31.536</f>
+        <f>ProcDataRM!K46*31.536</f>
         <v>15.768000000000001</v>
       </c>
     </row>
@@ -9520,14 +9602,14 @@
         <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D42" t="s">
         <v>16</v>
       </c>
       <c r="E42" t="str">
-        <f>ProcDataRM!B48</f>
-        <v>ERBIO-N</v>
+        <f>ProcDataRM!B47</f>
+        <v>ETGICEN-N</v>
       </c>
       <c r="F42" t="s">
         <v>11</v>
@@ -9542,15 +9624,15 @@
         <v>3</v>
       </c>
       <c r="R42">
-        <f>ProcDataRM!I48*31.536</f>
+        <f>ProcDataRM!I47*31.536</f>
         <v>15.768000000000001</v>
       </c>
       <c r="W42">
-        <f>ProcDataRM!J48*31.536</f>
+        <f>ProcDataRM!J47*31.536</f>
         <v>15.768000000000001</v>
       </c>
       <c r="AB42">
-        <f>ProcDataRM!K48*31.536</f>
+        <f>ProcDataRM!K47*31.536</f>
         <v>15.768000000000001</v>
       </c>
     </row>
@@ -9563,14 +9645,14 @@
         <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D43" t="s">
         <v>16</v>
       </c>
       <c r="E43" t="str">
-        <f>ProcDataRM!B49</f>
-        <v>ERBIG-N</v>
+        <f>ProcDataRM!B48</f>
+        <v>ERBIO-N</v>
       </c>
       <c r="F43" t="s">
         <v>11</v>
@@ -9585,15 +9667,15 @@
         <v>3</v>
       </c>
       <c r="R43">
-        <f>ProcDataRM!I49*31.536</f>
+        <f>ProcDataRM!I48*31.536</f>
         <v>15.768000000000001</v>
       </c>
       <c r="W43">
-        <f>ProcDataRM!J49*31.536</f>
+        <f>ProcDataRM!J48*31.536</f>
         <v>15.768000000000001</v>
       </c>
       <c r="AB43">
-        <f>ProcDataRM!K49*31.536</f>
+        <f>ProcDataRM!K48*31.536</f>
         <v>15.768000000000001</v>
       </c>
     </row>
@@ -9606,14 +9688,14 @@
         <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D44" t="s">
         <v>16</v>
       </c>
       <c r="E44" t="str">
-        <f>ProcDataRM!B50</f>
-        <v>ESTSUTL</v>
+        <f>ProcDataRM!B49</f>
+        <v>ERBIG-N</v>
       </c>
       <c r="F44" t="s">
         <v>11</v>
@@ -9627,32 +9709,36 @@
       <c r="I44">
         <v>3</v>
       </c>
-      <c r="W44" t="str">
-        <f>ProcDataRM!N50</f>
-        <v/>
-      </c>
-      <c r="AB44" t="str">
-        <f>ProcDataRM!O50</f>
-        <v/>
+      <c r="R44">
+        <f>ProcDataRM!I49*31.536</f>
+        <v>15.768000000000001</v>
+      </c>
+      <c r="W44">
+        <f>ProcDataRM!J49*31.536</f>
+        <v>15.768000000000001</v>
+      </c>
+      <c r="AB44">
+        <f>ProcDataRM!K49*31.536</f>
+        <v>15.768000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
         <f t="shared" si="2"/>
-        <v>*</v>
+        <v/>
       </c>
       <c r="B45" t="s">
         <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D45" t="s">
         <v>16</v>
       </c>
       <c r="E45" t="str">
-        <f>ProcDataRM!B51</f>
-        <v/>
+        <f>ProcDataRM!B50</f>
+        <v>ESTSUTL</v>
       </c>
       <c r="F45" t="s">
         <v>11</v>
@@ -9667,31 +9753,31 @@
         <v>3</v>
       </c>
       <c r="W45" t="str">
-        <f>ProcDataRM!N51</f>
+        <f>ProcDataRM!N50</f>
         <v/>
       </c>
       <c r="AB45" t="str">
-        <f>ProcDataRM!O51</f>
+        <f>ProcDataRM!O50</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>*</v>
       </c>
       <c r="B46" t="s">
         <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D46" t="s">
         <v>16</v>
       </c>
       <c r="E46" t="str">
-        <f>ProcDataRM!B52</f>
-        <v>ERSOLPRC-N</v>
+        <f>ProcDataRM!B51</f>
+        <v/>
       </c>
       <c r="F46" t="s">
         <v>11</v>
@@ -9706,11 +9792,11 @@
         <v>3</v>
       </c>
       <c r="W46" t="str">
-        <f>ProcDataRM!N52</f>
+        <f>ProcDataRM!N51</f>
         <v/>
       </c>
       <c r="AB46" t="str">
-        <f>ProcDataRM!O52</f>
+        <f>ProcDataRM!O51</f>
         <v/>
       </c>
     </row>
@@ -9723,14 +9809,14 @@
         <v>23</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D47" t="s">
         <v>16</v>
       </c>
       <c r="E47" t="str">
-        <f>ProcDataRM!B53</f>
-        <v>ERSOLPRR-N</v>
+        <f>ProcDataRM!B52</f>
+        <v>ERSOLPRC-N</v>
       </c>
       <c r="F47" t="s">
         <v>11</v>
@@ -9745,11 +9831,11 @@
         <v>3</v>
       </c>
       <c r="W47" t="str">
-        <f>ProcDataRM!N53</f>
+        <f>ProcDataRM!N52</f>
         <v/>
       </c>
       <c r="AB47" t="str">
-        <f>ProcDataRM!O53</f>
+        <f>ProcDataRM!O52</f>
         <v/>
       </c>
     </row>
@@ -9762,14 +9848,14 @@
         <v>23</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D48" t="s">
         <v>16</v>
       </c>
       <c r="E48" t="str">
-        <f>ProcDataRM!B54</f>
-        <v>ERSOLPRI-N</v>
+        <f>ProcDataRM!B53</f>
+        <v>ERSOLPRR-N</v>
       </c>
       <c r="F48" t="s">
         <v>11</v>
@@ -9784,11 +9870,11 @@
         <v>3</v>
       </c>
       <c r="W48" t="str">
-        <f>ProcDataRM!N54</f>
+        <f>ProcDataRM!N53</f>
         <v/>
       </c>
       <c r="AB48" t="str">
-        <f>ProcDataRM!O54</f>
+        <f>ProcDataRM!O53</f>
         <v/>
       </c>
     </row>
@@ -9801,14 +9887,14 @@
         <v>23</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D49" t="s">
         <v>16</v>
       </c>
       <c r="E49" t="str">
-        <f>ProcDataRM!B55</f>
-        <v>ETGASENSS-N</v>
+        <f>ProcDataRM!B54</f>
+        <v>ERSOLPRI-N</v>
       </c>
       <c r="F49" t="s">
         <v>11</v>
@@ -9823,11 +9909,11 @@
         <v>3</v>
       </c>
       <c r="W49" t="str">
-        <f>ProcDataRM!N55</f>
+        <f>ProcDataRM!N54</f>
         <v/>
       </c>
       <c r="AB49" t="str">
-        <f>ProcDataRM!O55</f>
+        <f>ProcDataRM!O54</f>
         <v/>
       </c>
     </row>
@@ -9840,14 +9926,14 @@
         <v>23</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D50" t="s">
         <v>16</v>
       </c>
       <c r="E50" t="str">
-        <f>ProcDataRM!B56</f>
-        <v>ETGASENSI-N</v>
+        <f>ProcDataRM!B55</f>
+        <v>ETGASENSS-N</v>
       </c>
       <c r="F50" t="s">
         <v>11</v>
@@ -9862,31 +9948,31 @@
         <v>3</v>
       </c>
       <c r="W50" t="str">
-        <f>ProcDataRM!N56</f>
+        <f>ProcDataRM!N55</f>
         <v/>
       </c>
       <c r="AB50" t="str">
-        <f>ProcDataRM!O56</f>
+        <f>ProcDataRM!O55</f>
         <v/>
       </c>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
         <f t="shared" si="2"/>
-        <v>*</v>
+        <v/>
       </c>
       <c r="B51" t="s">
         <v>23</v>
       </c>
       <c r="C51" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D51" t="s">
         <v>16</v>
       </c>
       <c r="E51" t="str">
-        <f>ProcDataRM!B57</f>
-        <v/>
+        <f>ProcDataRM!B56</f>
+        <v>ETGASENSI-N</v>
       </c>
       <c r="F51" t="s">
         <v>11</v>
@@ -9901,11 +9987,11 @@
         <v>3</v>
       </c>
       <c r="W51" t="str">
-        <f>ProcDataRM!N57</f>
+        <f>ProcDataRM!N56</f>
         <v/>
       </c>
       <c r="AB51" t="str">
-        <f>ProcDataRM!O57</f>
+        <f>ProcDataRM!O56</f>
         <v/>
       </c>
     </row>
@@ -9918,13 +10004,13 @@
         <v>23</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D52" t="s">
         <v>16</v>
       </c>
       <c r="E52" t="str">
-        <f>ProcDataRM!B58</f>
+        <f>ProcDataRM!B57</f>
         <v/>
       </c>
       <c r="F52" t="s">
@@ -9940,11 +10026,11 @@
         <v>3</v>
       </c>
       <c r="W52" t="str">
-        <f>ProcDataRM!N58</f>
+        <f>ProcDataRM!N57</f>
         <v/>
       </c>
       <c r="AB52" t="str">
-        <f>ProcDataRM!O58</f>
+        <f>ProcDataRM!O57</f>
         <v/>
       </c>
     </row>
@@ -9957,13 +10043,13 @@
         <v>23</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D53" t="s">
         <v>16</v>
       </c>
       <c r="E53" t="str">
-        <f>ProcDataRM!B59</f>
+        <f>ProcDataRM!B58</f>
         <v/>
       </c>
       <c r="F53" t="s">
@@ -9979,10 +10065,49 @@
         <v>3</v>
       </c>
       <c r="W53" t="str">
+        <f>ProcDataRM!N58</f>
+        <v/>
+      </c>
+      <c r="AB53" t="str">
+        <f>ProcDataRM!O58</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A54" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
+      </c>
+      <c r="B54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" t="str">
+        <f>ProcDataRM!B59</f>
+        <v/>
+      </c>
+      <c r="F54" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" t="s">
+        <v>11</v>
+      </c>
+      <c r="I54">
+        <v>3</v>
+      </c>
+      <c r="W54" t="str">
         <f>ProcDataRM!N59</f>
         <v/>
       </c>
-      <c r="AB53" t="str">
+      <c r="AB54" t="str">
         <f>ProcDataRM!O59</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Model Pre-DEFF presentation 1 on July 31
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/TCH_PWR_REL.xlsx
+++ b/SATIM/DataSpreadsheets/TCH_PWR_REL.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3460C40-9ED9-4E18-908A-30C9C54B9C4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81997EB5-1875-4087-A97F-02CF7FEBB04E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1155" yWindow="-17655" windowWidth="27555" windowHeight="13575" activeTab="6" xr2:uid="{7C70B42E-9201-48A9-B8F0-1466C79FDCED}"/>
-    <workbookView xWindow="570" yWindow="450" windowWidth="26880" windowHeight="13170" activeTab="4" xr2:uid="{C567A264-F0FD-49FD-BB9D-31E7FE2CFE51}"/>
   </bookViews>
   <sheets>
     <sheet name="ReserveMargin Inputs" sheetId="5" r:id="rId1"/>
@@ -1000,9 +999,9 @@
       <sheetName val="ANSv2-692-TS&amp;TID TRADE"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3">
         <row r="8">
           <cell r="A8" t="str">
@@ -1022,7 +1021,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7">
         <row r="9">
@@ -1031,10 +1030,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
       <sheetData sheetId="12">
         <row r="9">
           <cell r="B9" t="str">
@@ -2788,36 +2787,36 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
       <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3887,9 +3886,6 @@
   <dimension ref="B2:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3933,9 +3929,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4074,9 +4067,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4216,9 +4206,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10:AP10"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7737,9 +7724,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10:AP10"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10127,9 +10111,6 @@
     <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="AN2" sqref="AN2:AN3"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="E7" sqref="E7:E8"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10321,6 +10302,10 @@
         <f>4*5</f>
         <v>20</v>
       </c>
+      <c r="AM2">
+        <f>4.5*5</f>
+        <v>22.5</v>
+      </c>
       <c r="AN2">
         <f>5*3</f>
         <v>15</v>
@@ -10364,6 +10349,10 @@
       <c r="AL3">
         <f>4*5</f>
         <v>20</v>
+      </c>
+      <c r="AM3">
+        <f>4.5*5</f>
+        <v>22.5</v>
       </c>
       <c r="AN3">
         <f>5*3</f>
@@ -10534,9 +10523,6 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R9" sqref="R9"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="B41" sqref="B41:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>